<commit_message>
analyse file uitgebreid en input data vergroot
</commit_message>
<xml_diff>
--- a/mergesort OMP/Analyse omp.xlsx
+++ b/mergesort OMP/Analyse omp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nordi\Documents\4MA\PDS\Eindtaak\OMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nordi\Documents\4MA\PDS\PDS_ParallelizingSortingAlgos\mergesort OMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BED9348-CEF0-4DCF-B85D-49D752330410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4F3FFF-1952-44A1-AB8B-005867E12F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>speedup</t>
   </si>
@@ -54,15 +54,29 @@
   </si>
   <si>
     <t>efficiency</t>
+  </si>
+  <si>
+    <t>Merging serial</t>
+  </si>
+  <si>
+    <t>Merging parallel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -89,8 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -371,118 +388,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D2" t="e">
-        <f>B2/C2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F2" t="e">
-        <f>D2/E2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D3" t="e">
-        <f t="shared" ref="D3:D13" si="0">B3/C3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <f>B3/C3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3" t="e">
+        <f>D3/E3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3">
+        <f>A3</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>B3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" t="e">
+        <f>K3/L3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O3" t="e">
+        <f>M3/N3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="D4:D14" si="0">B4/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J13" si="1">A4</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K13" si="2">B4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" t="e">
+        <f t="shared" ref="M4:M13" si="3">K4/L4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M5" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M6" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D9" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M9" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D10" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D12" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>